<commit_message>
undo accidentall delete of all work
</commit_message>
<xml_diff>
--- a/Attack Balancing Sheet.xlsx
+++ b/Attack Balancing Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexw\OneDrive - Anglia Ruskin University\Year 1\Software Engineering for Games\VATS\STL\STL - Slower Than Light\STL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aw1204\UnityGames\STL-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360F29FE-46AE-4525-B72D-1813EA3206A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F61C41-EE8C-4208-B7CC-839AC177A5A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5340" windowWidth="29040" windowHeight="15720" xr2:uid="{A7FD60CB-5657-4ABB-B49D-7A8CAE78C830}"/>
+    <workbookView xWindow="105" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{A7FD60CB-5657-4ABB-B49D-7A8CAE78C830}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -80,9 +80,6 @@
     <t>max distance ~79.31</t>
   </si>
   <si>
-    <t>1-x^sqrt(sizeof component)</t>
-  </si>
-  <si>
     <t>ACCURACY CHART before factoring player accuracy</t>
   </si>
   <si>
@@ -159,6 +156,9 @@
   </si>
   <si>
     <t>beam</t>
+  </si>
+  <si>
+    <t>1-x^(0.4*sqrt(sizeof component))</t>
   </si>
 </sst>
 </file>
@@ -206,23 +206,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -231,14 +222,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2F3574A-1BE5-4723-978D-1D0EFA94D11D}">
   <dimension ref="A1:X46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,42 +583,42 @@
     <col min="4" max="4" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="H1" s="4" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D2" s="5" t="s">
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6" t="s">
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
       <c r="N2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D3" s="7" t="s">
+    <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
+      <c r="E3" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
       <c r="H3" s="9" t="s">
         <v>4</v>
       </c>
@@ -630,12 +629,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D4" s="10" t="s">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D4" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
@@ -646,8 +645,8 @@
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D5" s="10"/>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D5" s="6"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
@@ -656,51 +655,48 @@
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D7" s="10" t="s">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D8" s="6"/>
+      <c r="E8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="D8" s="10"/>
-      <c r="E8" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="Q10" s="13"/>
-    </row>
-    <row r="11" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+    </row>
+    <row r="11" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
       <c r="D11" t="s">
         <v>8</v>
       </c>
@@ -720,7 +716,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -749,7 +745,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>25.02</v>
       </c>
@@ -762,31 +758,31 @@
         <v>3.9976015988796298E-4</v>
       </c>
       <c r="D13" s="2">
-        <f>1-$C$13^SQRT(D12)</f>
-        <v>0.99960023984011204</v>
+        <f>1-$C$13^(0.4*SQRT(D12))</f>
+        <v>0.95627600821297809</v>
       </c>
       <c r="E13" s="2">
-        <f t="shared" ref="E13:I13" si="0">1-$C$13^SQRT(E12)</f>
-        <v>0.9999843606470995</v>
+        <f t="shared" ref="E13:I13" si="0">1-$C$13^(0.4*SQRT(E12))</f>
+        <v>0.98804120250416827</v>
       </c>
       <c r="F13" s="2">
         <f t="shared" si="0"/>
-        <v>0.99999869939895913</v>
+        <v>0.99557760389455829</v>
       </c>
       <c r="G13" s="2">
         <f t="shared" si="0"/>
-        <v>0.99999984019181454</v>
+        <v>0.99808821254220847</v>
       </c>
       <c r="H13" s="2">
         <f t="shared" si="0"/>
-        <v>0.99999997480045477</v>
+        <v>0.99908681854879999</v>
       </c>
       <c r="I13" s="2">
         <f t="shared" si="0"/>
-        <v>0.99999999525602101</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.99953177230021029</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>50</v>
       </c>
@@ -799,31 +795,31 @@
         <v>0.29289321881345254</v>
       </c>
       <c r="D14" s="2">
-        <f>1-$C$14^SQRT(D12)</f>
-        <v>0.70710678118654746</v>
+        <f>1-$C$14^(0.4*SQRT(D12))</f>
+        <v>0.38809538772894903</v>
       </c>
       <c r="E14" s="2">
-        <f t="shared" ref="E14:I14" si="2">1-$C$14^SQRT(E12)</f>
-        <v>0.82387821306335174</v>
+        <f t="shared" ref="E14:I14" si="2">1-$C$14^(0.4*SQRT(E12))</f>
+        <v>0.50074176935640646</v>
       </c>
       <c r="F14" s="2">
         <f t="shared" si="2"/>
-        <v>0.88078979315155448</v>
+        <v>0.57290412529742163</v>
       </c>
       <c r="G14" s="2">
         <f t="shared" si="2"/>
-        <v>0.91421356237309503</v>
+        <v>0.62557274548141484</v>
       </c>
       <c r="H14" s="2">
         <f t="shared" si="2"/>
-        <v>0.93580136699184002</v>
+        <v>0.66656566997598321</v>
       </c>
       <c r="I14" s="2">
         <f t="shared" si="2"/>
-        <v>0.95060193450003261</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.69974933589666066</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>79.31</v>
       </c>
@@ -836,718 +832,718 @@
         <v>0.43855653728919097</v>
       </c>
       <c r="D15" s="2">
-        <f>1-$C$15^SQRT(D12)</f>
-        <v>0.56144346271080903</v>
+        <f>1-$C$15^(0.4*SQRT(D12))</f>
+        <v>0.28086531550709204</v>
       </c>
       <c r="E15" s="2">
-        <f t="shared" ref="E15:I15" si="3">1-$C$15^SQRT(E12)</f>
-        <v>0.68829215460996385</v>
+        <f t="shared" ref="E15:I15" si="3">1-$C$15^(0.4*SQRT(E12))</f>
+        <v>0.37266561376978913</v>
       </c>
       <c r="F15" s="2">
         <f t="shared" si="3"/>
-        <v>0.76013320484061042</v>
+        <v>0.43507856576502024</v>
       </c>
       <c r="G15" s="2">
         <f t="shared" si="3"/>
-        <v>0.80766816360091442</v>
+        <v>0.48284530555928573</v>
       </c>
       <c r="H15" s="2">
         <f t="shared" si="3"/>
-        <v>0.84167668189758316</v>
+        <v>0.52157049689749768</v>
       </c>
       <c r="I15" s="2">
         <f t="shared" si="3"/>
-        <v>0.86721612070835974</v>
+        <v>0.55407877854554088</v>
       </c>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.25">
       <c r="M17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B18" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="12">
+      <c r="B18" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="7">
         <v>0.7</v>
       </c>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
     </row>
     <row r="19" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F19" s="12" t="s">
+      <c r="F19" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G19" s="12" t="s">
+      <c r="H19" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H19" s="12" t="s">
+      <c r="I19" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I19" s="12" t="s">
+      <c r="J19" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="J19" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="M19" s="12" t="s">
-        <v>34</v>
+      <c r="M19" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="U19" t="s">
+        <v>30</v>
+      </c>
+      <c r="V19" t="s">
         <v>31</v>
       </c>
-      <c r="V19" t="s">
+      <c r="W19" t="s">
         <v>32</v>
-      </c>
-      <c r="W19" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="20" spans="2:23" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="12">
-        <f>$E$18*D13</f>
-        <v>0.69972016788807834</v>
-      </c>
-      <c r="F20" s="12">
-        <f>$E$18*E13</f>
-        <v>0.69998905245296961</v>
-      </c>
-      <c r="G20" s="12">
-        <f>$E$18*F13</f>
-        <v>0.69999908957927137</v>
-      </c>
-      <c r="H20" s="12">
-        <f>$E$18*G13</f>
-        <v>0.69999988813427017</v>
-      </c>
-      <c r="I20" s="12">
-        <f>$E$18*H13</f>
-        <v>0.69999998236031824</v>
-      </c>
-      <c r="J20" s="12">
-        <f>$E$18*I13</f>
-        <v>0.69999999667921464</v>
+        <v>15</v>
+      </c>
+      <c r="E20" s="7">
+        <f t="shared" ref="E20:J20" si="4">$E$18*D13</f>
+        <v>0.66939320574908467</v>
+      </c>
+      <c r="F20" s="7">
+        <f t="shared" si="4"/>
+        <v>0.69162884175291772</v>
+      </c>
+      <c r="G20" s="7">
+        <f t="shared" si="4"/>
+        <v>0.69690432272619074</v>
+      </c>
+      <c r="H20" s="7">
+        <f t="shared" si="4"/>
+        <v>0.6986617487795459</v>
+      </c>
+      <c r="I20" s="7">
+        <f t="shared" si="4"/>
+        <v>0.69936077298416</v>
+      </c>
+      <c r="J20" s="7">
+        <f t="shared" si="4"/>
+        <v>0.69967224061014721</v>
       </c>
       <c r="M20" t="str">
         <f ca="1">IF(RAND()&gt;(1-E20),"yes","no")</f>
-        <v>no</v>
+        <v>yes</v>
       </c>
       <c r="N20" t="str">
-        <f t="shared" ref="N20:R20" ca="1" si="4">IF(RAND()&gt;(1-F20),"yes","no")</f>
-        <v>no</v>
+        <f t="shared" ref="N20:R20" ca="1" si="5">IF(RAND()&gt;(1-F20),"yes","no")</f>
+        <v>yes</v>
       </c>
       <c r="O20" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>yes</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>no</v>
       </c>
       <c r="P20" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>yes</v>
       </c>
       <c r="Q20" t="str">
-        <f t="shared" ca="1" si="4"/>
+        <f t="shared" ca="1" si="5"/>
         <v>yes</v>
       </c>
       <c r="R20" t="str">
-        <f t="shared" ca="1" si="4"/>
-        <v>yes</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>no</v>
       </c>
       <c r="T20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U20">
         <f ca="1">COUNTIF(M20:R22,"yes")</f>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="V20">
         <f ca="1">COUNTIF(M20:R22,"no")</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="W20">
-        <f t="shared" ref="W20:W22" ca="1" si="5">U20/(U20+V20)*100</f>
-        <v>66.666666666666657</v>
+        <f t="shared" ref="W20:W22" ca="1" si="6">U20/(U20+V20)*100</f>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="2:23" x14ac:dyDescent="0.25">
       <c r="D21" t="s">
-        <v>17</v>
-      </c>
-      <c r="E21" s="12">
-        <f t="shared" ref="E21:J21" si="6">$E$18*D14</f>
-        <v>0.49497474683058318</v>
-      </c>
-      <c r="F21" s="12">
-        <f t="shared" si="6"/>
-        <v>0.57671474914434617</v>
-      </c>
-      <c r="G21" s="12">
-        <f t="shared" si="6"/>
-        <v>0.61655285520608805</v>
-      </c>
-      <c r="H21" s="12">
-        <f t="shared" si="6"/>
-        <v>0.63994949366116649</v>
-      </c>
-      <c r="I21" s="12">
-        <f t="shared" si="6"/>
-        <v>0.655060956894288</v>
-      </c>
-      <c r="J21" s="12">
-        <f t="shared" si="6"/>
-        <v>0.66542135415002279</v>
+        <v>16</v>
+      </c>
+      <c r="E21" s="7">
+        <f t="shared" ref="E21:J21" si="7">$E$18*D14</f>
+        <v>0.2716667714102643</v>
+      </c>
+      <c r="F21" s="7">
+        <f t="shared" si="7"/>
+        <v>0.35051923854948452</v>
+      </c>
+      <c r="G21" s="7">
+        <f t="shared" si="7"/>
+        <v>0.40103288770819512</v>
+      </c>
+      <c r="H21" s="7">
+        <f t="shared" si="7"/>
+        <v>0.43790092183699036</v>
+      </c>
+      <c r="I21" s="7">
+        <f t="shared" si="7"/>
+        <v>0.46659596898318823</v>
+      </c>
+      <c r="J21" s="7">
+        <f t="shared" si="7"/>
+        <v>0.48982453512766244</v>
       </c>
       <c r="M21" t="str">
-        <f t="shared" ref="M21:M23" ca="1" si="7">IF(RAND()&gt;(1-E21),"yes","no")</f>
-        <v>yes</v>
+        <f t="shared" ref="M21:M22" ca="1" si="8">IF(RAND()&gt;(1-E21),"yes","no")</f>
+        <v>no</v>
       </c>
       <c r="N21" t="str">
-        <f t="shared" ref="N21:N23" ca="1" si="8">IF(RAND()&gt;(1-F21),"yes","no")</f>
-        <v>no</v>
+        <f t="shared" ref="N21:N22" ca="1" si="9">IF(RAND()&gt;(1-F21),"yes","no")</f>
+        <v>yes</v>
       </c>
       <c r="O21" t="str">
-        <f t="shared" ref="O21:O23" ca="1" si="9">IF(RAND()&gt;(1-G21),"yes","no")</f>
+        <f t="shared" ref="O21:O22" ca="1" si="10">IF(RAND()&gt;(1-G21),"yes","no")</f>
         <v>no</v>
       </c>
       <c r="P21" t="str">
-        <f t="shared" ref="P21:P23" ca="1" si="10">IF(RAND()&gt;(1-H21),"yes","no")</f>
-        <v>yes</v>
+        <f t="shared" ref="P21:P22" ca="1" si="11">IF(RAND()&gt;(1-H21),"yes","no")</f>
+        <v>no</v>
       </c>
       <c r="Q21" t="str">
-        <f t="shared" ref="Q21:Q23" ca="1" si="11">IF(RAND()&gt;(1-I21),"yes","no")</f>
-        <v>yes</v>
+        <f t="shared" ref="Q21:Q22" ca="1" si="12">IF(RAND()&gt;(1-I21),"yes","no")</f>
+        <v>no</v>
       </c>
       <c r="R21" t="str">
-        <f t="shared" ref="R21:R23" ca="1" si="12">IF(RAND()&gt;(1-J21),"yes","no")</f>
-        <v>yes</v>
+        <f t="shared" ref="R21:R22" ca="1" si="13">IF(RAND()&gt;(1-J21),"yes","no")</f>
+        <v>no</v>
       </c>
       <c r="T21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="U21">
         <f ca="1">COUNTIF(M26:R28,"yes")</f>
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="V21">
         <f ca="1">COUNTIF(M26:R28,"no")</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="W21">
-        <f t="shared" ca="1" si="5"/>
-        <v>88.888888888888886</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>66.666666666666657</v>
       </c>
     </row>
     <row r="22" spans="2:23" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" s="12">
-        <f t="shared" ref="E22:J22" si="13">$E$18*D15</f>
-        <v>0.3930104238975663</v>
-      </c>
-      <c r="F22" s="12">
-        <f t="shared" si="13"/>
-        <v>0.48180450822697468</v>
-      </c>
-      <c r="G22" s="12">
-        <f t="shared" si="13"/>
-        <v>0.53209324338842723</v>
-      </c>
-      <c r="H22" s="12">
-        <f t="shared" si="13"/>
-        <v>0.56536771452064005</v>
-      </c>
-      <c r="I22" s="12">
-        <f t="shared" si="13"/>
-        <v>0.58917367732830817</v>
-      </c>
-      <c r="J22" s="12">
-        <f t="shared" si="13"/>
-        <v>0.60705128449585177</v>
+        <v>17</v>
+      </c>
+      <c r="E22" s="7">
+        <f t="shared" ref="E22:J22" si="14">$E$18*D15</f>
+        <v>0.19660572085496442</v>
+      </c>
+      <c r="F22" s="7">
+        <f t="shared" si="14"/>
+        <v>0.26086592963885236</v>
+      </c>
+      <c r="G22" s="7">
+        <f t="shared" si="14"/>
+        <v>0.30455499603551417</v>
+      </c>
+      <c r="H22" s="7">
+        <f t="shared" si="14"/>
+        <v>0.33799171389150001</v>
+      </c>
+      <c r="I22" s="7">
+        <f t="shared" si="14"/>
+        <v>0.36509934782824838</v>
+      </c>
+      <c r="J22" s="7">
+        <f t="shared" si="14"/>
+        <v>0.38785514498187862</v>
       </c>
       <c r="M22" t="str">
-        <f t="shared" ca="1" si="7"/>
+        <f t="shared" ca="1" si="8"/>
         <v>no</v>
       </c>
       <c r="N22" t="str">
-        <f t="shared" ca="1" si="8"/>
-        <v>no</v>
+        <f t="shared" ca="1" si="9"/>
+        <v>yes</v>
       </c>
       <c r="O22" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" ca="1" si="10"/>
         <v>yes</v>
       </c>
       <c r="P22" t="str">
-        <f t="shared" ca="1" si="10"/>
-        <v>yes</v>
+        <f t="shared" ca="1" si="11"/>
+        <v>no</v>
       </c>
       <c r="Q22" t="str">
-        <f t="shared" ca="1" si="11"/>
+        <f t="shared" ca="1" si="12"/>
         <v>yes</v>
       </c>
       <c r="R22" t="str">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>yes</v>
       </c>
       <c r="T22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="U22">
         <f ca="1">COUNTIF(M32:R34,"yes")</f>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="V22">
         <f ca="1">COUNTIF(M32:R34,"no")</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="W22">
-        <f t="shared" ca="1" si="5"/>
-        <v>83.333333333333343</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>61.111111111111114</v>
       </c>
     </row>
     <row r="23" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
       <c r="T23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U23">
         <f ca="1">COUNTIF(M20:R34,"yes")</f>
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="V23">
         <f ca="1">COUNTIF(M20:R34,"no")</f>
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="W23">
         <f ca="1">U23/(U23+V23)*100</f>
-        <v>79.629629629629633</v>
+        <v>59.259259259259252</v>
       </c>
     </row>
     <row r="24" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="12">
+      <c r="B24" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="7">
         <v>0.9</v>
       </c>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
     </row>
     <row r="25" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="12" t="s">
+      <c r="E25" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F25" s="12" t="s">
+      <c r="F25" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G25" s="12" t="s">
+      <c r="H25" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H25" s="12" t="s">
+      <c r="I25" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I25" s="12" t="s">
+      <c r="J25" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="J25" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="M25" s="12" t="s">
-        <v>35</v>
+      <c r="M25" s="7" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="2:23" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>16</v>
-      </c>
-      <c r="E26" s="12">
+        <v>15</v>
+      </c>
+      <c r="E26" s="7">
         <f>$E$24*D13</f>
-        <v>0.89964021585610088</v>
-      </c>
-      <c r="F26" s="12">
-        <f t="shared" ref="F26:J26" si="14">$E$24*E13</f>
-        <v>0.89998592458238957</v>
-      </c>
-      <c r="G26" s="12">
-        <f t="shared" si="14"/>
-        <v>0.89999882945906329</v>
-      </c>
-      <c r="H26" s="12">
-        <f t="shared" si="14"/>
-        <v>0.89999985617263312</v>
-      </c>
-      <c r="I26" s="12">
-        <f t="shared" si="14"/>
-        <v>0.89999997732040926</v>
-      </c>
-      <c r="J26" s="12">
-        <f t="shared" si="14"/>
-        <v>0.89999999573041889</v>
+        <v>0.86064840739168025</v>
+      </c>
+      <c r="F26" s="7">
+        <f t="shared" ref="F26:J26" si="15">$E$24*E13</f>
+        <v>0.88923708225375142</v>
+      </c>
+      <c r="G26" s="7">
+        <f t="shared" si="15"/>
+        <v>0.89601984350510244</v>
+      </c>
+      <c r="H26" s="7">
+        <f t="shared" si="15"/>
+        <v>0.89827939128798762</v>
+      </c>
+      <c r="I26" s="7">
+        <f t="shared" si="15"/>
+        <v>0.89917813669391999</v>
+      </c>
+      <c r="J26" s="7">
+        <f t="shared" si="15"/>
+        <v>0.89957859507018934</v>
       </c>
       <c r="M26" t="str">
-        <f t="shared" ref="M24:M34" ca="1" si="15">IF(RAND()&gt;(1-E26),"yes","no")</f>
+        <f t="shared" ref="M26:M34" ca="1" si="16">IF(RAND()&gt;(1-E26),"yes","no")</f>
         <v>yes</v>
       </c>
       <c r="N26" t="str">
-        <f t="shared" ref="N24:N34" ca="1" si="16">IF(RAND()&gt;(1-F26),"yes","no")</f>
+        <f t="shared" ref="N26:N34" ca="1" si="17">IF(RAND()&gt;(1-F26),"yes","no")</f>
         <v>yes</v>
       </c>
       <c r="O26" t="str">
-        <f t="shared" ref="O24:O34" ca="1" si="17">IF(RAND()&gt;(1-G26),"yes","no")</f>
+        <f t="shared" ref="O26:O34" ca="1" si="18">IF(RAND()&gt;(1-G26),"yes","no")</f>
         <v>yes</v>
       </c>
       <c r="P26" t="str">
-        <f t="shared" ref="P24:P34" ca="1" si="18">IF(RAND()&gt;(1-H26),"yes","no")</f>
+        <f t="shared" ref="P26:P34" ca="1" si="19">IF(RAND()&gt;(1-H26),"yes","no")</f>
         <v>yes</v>
       </c>
       <c r="Q26" t="str">
-        <f t="shared" ref="Q24:Q34" ca="1" si="19">IF(RAND()&gt;(1-I26),"yes","no")</f>
+        <f t="shared" ref="Q26:Q34" ca="1" si="20">IF(RAND()&gt;(1-I26),"yes","no")</f>
         <v>yes</v>
       </c>
       <c r="R26" t="str">
-        <f t="shared" ref="R24:R34" ca="1" si="20">IF(RAND()&gt;(1-J26),"yes","no")</f>
+        <f t="shared" ref="R26:R34" ca="1" si="21">IF(RAND()&gt;(1-J26),"yes","no")</f>
         <v>yes</v>
       </c>
     </row>
     <row r="27" spans="2:23" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
-        <v>17</v>
-      </c>
-      <c r="E27" s="12">
-        <f t="shared" ref="E27:J27" si="21">$E$24*D14</f>
-        <v>0.63639610306789274</v>
-      </c>
-      <c r="F27" s="12">
-        <f t="shared" si="21"/>
-        <v>0.74149039175701659</v>
-      </c>
-      <c r="G27" s="12">
-        <f t="shared" si="21"/>
-        <v>0.79271081383639908</v>
-      </c>
-      <c r="H27" s="12">
-        <f t="shared" si="21"/>
-        <v>0.82279220613578552</v>
-      </c>
-      <c r="I27" s="12">
-        <f t="shared" si="21"/>
-        <v>0.84222123029265605</v>
-      </c>
-      <c r="J27" s="12">
-        <f t="shared" si="21"/>
-        <v>0.85554174105002934</v>
+        <v>16</v>
+      </c>
+      <c r="E27" s="7">
+        <f t="shared" ref="E27:J27" si="22">$E$24*D14</f>
+        <v>0.34928584895605413</v>
+      </c>
+      <c r="F27" s="7">
+        <f t="shared" si="22"/>
+        <v>0.45066759242076582</v>
+      </c>
+      <c r="G27" s="7">
+        <f t="shared" si="22"/>
+        <v>0.51561371276767953</v>
+      </c>
+      <c r="H27" s="7">
+        <f t="shared" si="22"/>
+        <v>0.56301547093327342</v>
+      </c>
+      <c r="I27" s="7">
+        <f t="shared" si="22"/>
+        <v>0.59990910297838496</v>
+      </c>
+      <c r="J27" s="7">
+        <f t="shared" si="22"/>
+        <v>0.62977440230699466</v>
       </c>
       <c r="M27" t="str">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="16"/>
         <v>yes</v>
       </c>
       <c r="N27" t="str">
-        <f t="shared" ca="1" si="16"/>
-        <v>yes</v>
+        <f t="shared" ca="1" si="17"/>
+        <v>no</v>
       </c>
       <c r="O27" t="str">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="18"/>
         <v>yes</v>
       </c>
       <c r="P27" t="str">
-        <f t="shared" ca="1" si="18"/>
-        <v>yes</v>
+        <f t="shared" ca="1" si="19"/>
+        <v>no</v>
       </c>
       <c r="Q27" t="str">
-        <f t="shared" ca="1" si="19"/>
-        <v>no</v>
+        <f t="shared" ca="1" si="20"/>
+        <v>yes</v>
       </c>
       <c r="R27" t="str">
-        <f t="shared" ca="1" si="20"/>
-        <v>yes</v>
+        <f t="shared" ca="1" si="21"/>
+        <v>no</v>
       </c>
     </row>
     <row r="28" spans="2:23" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
-        <v>18</v>
-      </c>
-      <c r="E28" s="12">
-        <f t="shared" ref="E28:J28" si="22">$E$24*D15</f>
-        <v>0.50529911643972814</v>
-      </c>
-      <c r="F28" s="12">
-        <f t="shared" si="22"/>
-        <v>0.61946293914896744</v>
-      </c>
-      <c r="G28" s="12">
-        <f t="shared" si="22"/>
-        <v>0.68411988435654936</v>
-      </c>
-      <c r="H28" s="12">
-        <f t="shared" si="22"/>
-        <v>0.726901347240823</v>
-      </c>
-      <c r="I28" s="12">
-        <f t="shared" si="22"/>
-        <v>0.75750901370782486</v>
-      </c>
-      <c r="J28" s="12">
-        <f t="shared" si="22"/>
-        <v>0.78049450863752379</v>
+        <v>17</v>
+      </c>
+      <c r="E28" s="7">
+        <f t="shared" ref="E28:J28" si="23">$E$24*D15</f>
+        <v>0.25277878395638287</v>
+      </c>
+      <c r="F28" s="7">
+        <f t="shared" si="23"/>
+        <v>0.3353990523928102</v>
+      </c>
+      <c r="G28" s="7">
+        <f t="shared" si="23"/>
+        <v>0.39157070918851822</v>
+      </c>
+      <c r="H28" s="7">
+        <f t="shared" si="23"/>
+        <v>0.43456077500335716</v>
+      </c>
+      <c r="I28" s="7">
+        <f t="shared" si="23"/>
+        <v>0.46941344720774791</v>
+      </c>
+      <c r="J28" s="7">
+        <f t="shared" si="23"/>
+        <v>0.4986709006909868</v>
       </c>
       <c r="M28" t="str">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="16"/>
         <v>yes</v>
       </c>
       <c r="N28" t="str">
-        <f t="shared" ca="1" si="16"/>
-        <v>yes</v>
+        <f t="shared" ca="1" si="17"/>
+        <v>no</v>
       </c>
       <c r="O28" t="str">
-        <f t="shared" ca="1" si="17"/>
-        <v>yes</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>no</v>
       </c>
       <c r="P28" t="str">
-        <f t="shared" ca="1" si="18"/>
-        <v>no</v>
+        <f t="shared" ca="1" si="19"/>
+        <v>yes</v>
       </c>
       <c r="Q28" t="str">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="20"/>
         <v>yes</v>
       </c>
       <c r="R28" t="str">
-        <f t="shared" ca="1" si="20"/>
-        <v>yes</v>
+        <f t="shared" ca="1" si="21"/>
+        <v>no</v>
       </c>
     </row>
     <row r="29" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="12"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
     </row>
     <row r="30" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B30" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="12">
+      <c r="B30" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="7">
         <v>0.95</v>
       </c>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="12"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
     </row>
     <row r="31" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
-      <c r="E31" s="12" t="s">
+      <c r="E31" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F31" s="12" t="s">
+      <c r="F31" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G31" s="12" t="s">
+      <c r="H31" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H31" s="12" t="s">
+      <c r="I31" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="I31" s="12" t="s">
+      <c r="J31" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="J31" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="M31" s="12" t="s">
-        <v>35</v>
+      <c r="M31" s="7" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="2:23" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
-        <v>16</v>
-      </c>
-      <c r="E32" s="12">
+        <v>15</v>
+      </c>
+      <c r="E32" s="7">
         <f>$E$30*D13</f>
-        <v>0.9496202278481064</v>
-      </c>
-      <c r="F32" s="12">
-        <f t="shared" ref="F32:J32" si="23">$E$30*E13</f>
-        <v>0.94998514261474454</v>
-      </c>
-      <c r="G32" s="12">
-        <f t="shared" si="23"/>
-        <v>0.9499987644290111</v>
-      </c>
-      <c r="H32" s="12">
-        <f t="shared" si="23"/>
-        <v>0.94999984818222372</v>
-      </c>
-      <c r="I32" s="12">
-        <f t="shared" si="23"/>
-        <v>0.94999997606043196</v>
-      </c>
-      <c r="J32" s="12">
-        <f t="shared" si="23"/>
-        <v>0.9499999954932199</v>
+        <v>0.90846220780232911</v>
+      </c>
+      <c r="F32" s="7">
+        <f t="shared" ref="F32:J32" si="24">$E$30*E13</f>
+        <v>0.93863914237895985</v>
+      </c>
+      <c r="G32" s="7">
+        <f t="shared" si="24"/>
+        <v>0.94579872369983031</v>
+      </c>
+      <c r="H32" s="7">
+        <f t="shared" si="24"/>
+        <v>0.94818380191509799</v>
+      </c>
+      <c r="I32" s="7">
+        <f t="shared" si="24"/>
+        <v>0.94913247762135999</v>
+      </c>
+      <c r="J32" s="7">
+        <f t="shared" si="24"/>
+        <v>0.94955518368519976</v>
       </c>
       <c r="M32" t="str">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="16"/>
         <v>yes</v>
       </c>
       <c r="N32" t="str">
-        <f t="shared" ca="1" si="16"/>
-        <v>yes</v>
+        <f t="shared" ca="1" si="17"/>
+        <v>no</v>
       </c>
       <c r="O32" t="str">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="18"/>
         <v>yes</v>
       </c>
       <c r="P32" t="str">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="19"/>
         <v>yes</v>
       </c>
       <c r="Q32" t="str">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="20"/>
         <v>yes</v>
       </c>
       <c r="R32" t="str">
-        <f t="shared" ca="1" si="20"/>
+        <f t="shared" ca="1" si="21"/>
         <v>yes</v>
       </c>
     </row>
     <row r="33" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>17</v>
-      </c>
-      <c r="E33" s="12">
-        <f t="shared" ref="E33:J33" si="24">$E$30*D14</f>
-        <v>0.67175144212722004</v>
-      </c>
-      <c r="F33" s="12">
-        <f t="shared" si="24"/>
-        <v>0.78268430241018416</v>
-      </c>
-      <c r="G33" s="12">
-        <f t="shared" si="24"/>
-        <v>0.83675030349397672</v>
-      </c>
-      <c r="H33" s="12">
-        <f t="shared" si="24"/>
-        <v>0.86850288425444022</v>
-      </c>
-      <c r="I33" s="12">
-        <f t="shared" si="24"/>
-        <v>0.88901129864224793</v>
-      </c>
-      <c r="J33" s="12">
-        <f t="shared" si="24"/>
-        <v>0.90307183777503097</v>
+        <v>16</v>
+      </c>
+      <c r="E33" s="7">
+        <f t="shared" ref="E33:J33" si="25">$E$30*D14</f>
+        <v>0.36869061834250155</v>
+      </c>
+      <c r="F33" s="7">
+        <f t="shared" si="25"/>
+        <v>0.47570468088858614</v>
+      </c>
+      <c r="G33" s="7">
+        <f t="shared" si="25"/>
+        <v>0.54425891903255053</v>
+      </c>
+      <c r="H33" s="7">
+        <f t="shared" si="25"/>
+        <v>0.59429410820734407</v>
+      </c>
+      <c r="I33" s="7">
+        <f t="shared" si="25"/>
+        <v>0.63323738647718397</v>
+      </c>
+      <c r="J33" s="7">
+        <f t="shared" si="25"/>
+        <v>0.66476186910182755</v>
       </c>
       <c r="M33" t="str">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="16"/>
         <v>yes</v>
       </c>
       <c r="N33" t="str">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="17"/>
         <v>yes</v>
       </c>
       <c r="O33" t="str">
-        <f t="shared" ca="1" si="17"/>
-        <v>yes</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>no</v>
       </c>
       <c r="P33" t="str">
-        <f t="shared" ca="1" si="18"/>
-        <v>yes</v>
+        <f t="shared" ca="1" si="19"/>
+        <v>no</v>
       </c>
       <c r="Q33" t="str">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="20"/>
         <v>yes</v>
       </c>
       <c r="R33" t="str">
-        <f t="shared" ca="1" si="20"/>
+        <f t="shared" ca="1" si="21"/>
         <v>yes</v>
       </c>
     </row>
     <row r="34" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>18</v>
-      </c>
-      <c r="E34" s="12">
-        <f t="shared" ref="E34:J34" si="25">$E$30*D15</f>
-        <v>0.53337128957526858</v>
-      </c>
-      <c r="F34" s="12">
-        <f t="shared" si="25"/>
-        <v>0.65387754687946564</v>
-      </c>
-      <c r="G34" s="12">
-        <f t="shared" si="25"/>
-        <v>0.72212654459857983</v>
-      </c>
-      <c r="H34" s="12">
-        <f t="shared" si="25"/>
-        <v>0.76728475542086871</v>
-      </c>
-      <c r="I34" s="12">
-        <f t="shared" si="25"/>
-        <v>0.79959284780270401</v>
-      </c>
-      <c r="J34" s="12">
-        <f t="shared" si="25"/>
-        <v>0.82385531467294171</v>
+        <v>17</v>
+      </c>
+      <c r="E34" s="7">
+        <f t="shared" ref="E34:J34" si="26">$E$30*D15</f>
+        <v>0.2668220497317374</v>
+      </c>
+      <c r="F34" s="7">
+        <f t="shared" si="26"/>
+        <v>0.35403233308129967</v>
+      </c>
+      <c r="G34" s="7">
+        <f t="shared" si="26"/>
+        <v>0.41332463747676923</v>
+      </c>
+      <c r="H34" s="7">
+        <f t="shared" si="26"/>
+        <v>0.45870304028132142</v>
+      </c>
+      <c r="I34" s="7">
+        <f t="shared" si="26"/>
+        <v>0.4954919720526228</v>
+      </c>
+      <c r="J34" s="7">
+        <f t="shared" si="26"/>
+        <v>0.52637483961826381</v>
       </c>
       <c r="M34" t="str">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="16"/>
         <v>no</v>
       </c>
       <c r="N34" t="str">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="17"/>
         <v>no</v>
       </c>
       <c r="O34" t="str">
-        <f t="shared" ca="1" si="17"/>
-        <v>yes</v>
+        <f t="shared" ca="1" si="18"/>
+        <v>no</v>
       </c>
       <c r="P34" t="str">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="19"/>
         <v>yes</v>
       </c>
       <c r="Q34" t="str">
-        <f t="shared" ca="1" si="19"/>
-        <v>no</v>
+        <f t="shared" ca="1" si="20"/>
+        <v>yes</v>
       </c>
       <c r="R34" t="str">
-        <f t="shared" ca="1" si="20"/>
-        <v>yes</v>
+        <f t="shared" ca="1" si="21"/>
+        <v>no</v>
       </c>
     </row>
     <row r="46" spans="4:24" x14ac:dyDescent="0.25">
@@ -1557,6 +1553,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
     <mergeCell ref="B30:D30"/>
     <mergeCell ref="H3:K3"/>
     <mergeCell ref="H4:K4"/>
@@ -1564,11 +1565,6 @@
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="B24:D24"/>
-    <mergeCell ref="H1:K1"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:G4"/>
     <mergeCell ref="E5:G5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
commented code and added in refeerences for third party researching
</commit_message>
<xml_diff>
--- a/Attack Balancing Sheet.xlsx
+++ b/Attack Balancing Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aw1204\UnityGames\STL-main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://myaru-my.sharepoint.com/personal/aw1204_student_aru_ac_uk/Documents/Year 1/Software Engineering for Games/VATS/STL/STL - Slower Than Light/STL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F61C41-EE8C-4208-B7CC-839AC177A5A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{B3F61C41-EE8C-4208-B7CC-839AC177A5A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EECD41F3-0060-4A7A-BCBB-53C2C7BD4613}"/>
   <bookViews>
-    <workbookView xWindow="105" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{A7FD60CB-5657-4ABB-B49D-7A8CAE78C830}"/>
+    <workbookView xWindow="38280" yWindow="5340" windowWidth="29040" windowHeight="15720" xr2:uid="{A7FD60CB-5657-4ABB-B49D-7A8CAE78C830}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
   <si>
     <t>x=</t>
   </si>
@@ -50,9 +50,6 @@
     <t>dist</t>
   </si>
   <si>
-    <t>dist,size</t>
-  </si>
-  <si>
     <t>1-1/sqrt(dist)*5</t>
   </si>
   <si>
@@ -65,9 +62,6 @@
     <t>size</t>
   </si>
   <si>
-    <t>dist,size,acc</t>
-  </si>
-  <si>
     <t>w</t>
   </si>
   <si>
@@ -119,9 +113,6 @@
     <t>Accuracy with Beam :</t>
   </si>
   <si>
-    <t>isHit</t>
-  </si>
-  <si>
     <t xml:space="preserve">roll RNG up to 100, </t>
   </si>
   <si>
@@ -159,16 +150,35 @@
   </si>
   <si>
     <t>1-x^(0.4*sqrt(sizeof component))</t>
+  </si>
+  <si>
+    <t>isHit=</t>
+  </si>
+  <si>
+    <t>distance</t>
+  </si>
+  <si>
+    <t>dist, size</t>
+  </si>
+  <si>
+    <t>dist, size, acc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -206,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -226,18 +236,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,7 +586,7 @@
   <dimension ref="A1:X46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:G4"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,67 +604,67 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D2" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
+        <v>9</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
       <c r="N2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
       <c r="N3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
+      <c r="E4" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D5" s="6"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D6" s="6"/>
@@ -667,10 +678,10 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D7" s="6" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -682,7 +693,7 @@
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D8" s="6"/>
       <c r="E8" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
@@ -691,29 +702,35 @@
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
     </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="13" t="str">
+        <f>"//below chart represents normalised values for the accuracy equation"</f>
+        <v>//below chart represents normalised values for the accuracy equation</v>
+      </c>
+    </row>
     <row r="11" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
+      <c r="A11" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -721,10 +738,10 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -856,14 +873,18 @@
         <v>0.55407877854554088</v>
       </c>
     </row>
-    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="C17" s="13" t="str">
+        <f>"//the below applies the eqation's logic to the different accuracy values of different weapons"</f>
+        <v>//the below applies the eqation's logic to the different accuracy values of different weapons</v>
+      </c>
       <c r="M17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
@@ -875,45 +896,44 @@
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
-    </row>
-    <row r="19" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="M18" s="13" t="str">
+        <f>"// rolls against the respective odds in the table to the left to simulate a round of attacks"</f>
+        <v>// rolls against the respective odds in the table to the left to simulate a round of attacks</v>
+      </c>
+    </row>
+    <row r="19" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F19" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="I19" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H19" s="7" t="s">
+      <c r="J19" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I19" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>22</v>
-      </c>
       <c r="M19" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="U19" t="s">
         <v>30</v>
       </c>
-      <c r="V19" t="s">
-        <v>31</v>
-      </c>
-      <c r="W19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="U19" s="13" t="str">
+        <f>"//counts the intstances of successful hits  "</f>
+        <v xml:space="preserve">//counts the intstances of successful hits  </v>
+      </c>
+    </row>
+    <row r="20" spans="2:24" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E20" s="7">
         <f t="shared" ref="E20:J20" si="4">$E$18*D13</f>
@@ -941,7 +961,7 @@
       </c>
       <c r="M20" t="str">
         <f ca="1">IF(RAND()&gt;(1-E20),"yes","no")</f>
-        <v>yes</v>
+        <v>no</v>
       </c>
       <c r="N20" t="str">
         <f t="shared" ref="N20:R20" ca="1" si="5">IF(RAND()&gt;(1-F20),"yes","no")</f>
@@ -961,95 +981,89 @@
       </c>
       <c r="R20" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>no</v>
-      </c>
-      <c r="T20" t="s">
-        <v>37</v>
-      </c>
-      <c r="U20">
+        <v>yes</v>
+      </c>
+      <c r="V20" t="s">
+        <v>27</v>
+      </c>
+      <c r="W20" t="s">
+        <v>28</v>
+      </c>
+      <c r="X20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="7">
+        <f t="shared" ref="E21:J21" si="6">$E$18*D14</f>
+        <v>0.2716667714102643</v>
+      </c>
+      <c r="F21" s="7">
+        <f t="shared" si="6"/>
+        <v>0.35051923854948452</v>
+      </c>
+      <c r="G21" s="7">
+        <f t="shared" si="6"/>
+        <v>0.40103288770819512</v>
+      </c>
+      <c r="H21" s="7">
+        <f t="shared" si="6"/>
+        <v>0.43790092183699036</v>
+      </c>
+      <c r="I21" s="7">
+        <f t="shared" si="6"/>
+        <v>0.46659596898318823</v>
+      </c>
+      <c r="J21" s="7">
+        <f t="shared" si="6"/>
+        <v>0.48982453512766244</v>
+      </c>
+      <c r="M21" t="str">
+        <f t="shared" ref="M21:M22" ca="1" si="7">IF(RAND()&gt;(1-E21),"yes","no")</f>
+        <v>no</v>
+      </c>
+      <c r="N21" t="str">
+        <f t="shared" ref="N21:N22" ca="1" si="8">IF(RAND()&gt;(1-F21),"yes","no")</f>
+        <v>no</v>
+      </c>
+      <c r="O21" t="str">
+        <f t="shared" ref="O21:O22" ca="1" si="9">IF(RAND()&gt;(1-G21),"yes","no")</f>
+        <v>no</v>
+      </c>
+      <c r="P21" t="str">
+        <f t="shared" ref="P21:P22" ca="1" si="10">IF(RAND()&gt;(1-H21),"yes","no")</f>
+        <v>no</v>
+      </c>
+      <c r="Q21" t="str">
+        <f t="shared" ref="Q21:Q22" ca="1" si="11">IF(RAND()&gt;(1-I21),"yes","no")</f>
+        <v>yes</v>
+      </c>
+      <c r="R21" t="str">
+        <f t="shared" ref="R21:R22" ca="1" si="12">IF(RAND()&gt;(1-J21),"yes","no")</f>
+        <v>no</v>
+      </c>
+      <c r="U21" t="s">
+        <v>34</v>
+      </c>
+      <c r="V21">
         <f ca="1">COUNTIF(M20:R22,"yes")</f>
-        <v>9</v>
-      </c>
-      <c r="V20">
+        <v>6</v>
+      </c>
+      <c r="W21">
         <f ca="1">COUNTIF(M20:R22,"no")</f>
-        <v>9</v>
-      </c>
-      <c r="W20">
-        <f t="shared" ref="W20:W22" ca="1" si="6">U20/(U20+V20)*100</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="D21" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="7">
-        <f t="shared" ref="E21:J21" si="7">$E$18*D14</f>
-        <v>0.2716667714102643</v>
-      </c>
-      <c r="F21" s="7">
-        <f t="shared" si="7"/>
-        <v>0.35051923854948452</v>
-      </c>
-      <c r="G21" s="7">
-        <f t="shared" si="7"/>
-        <v>0.40103288770819512</v>
-      </c>
-      <c r="H21" s="7">
-        <f t="shared" si="7"/>
-        <v>0.43790092183699036</v>
-      </c>
-      <c r="I21" s="7">
-        <f t="shared" si="7"/>
-        <v>0.46659596898318823</v>
-      </c>
-      <c r="J21" s="7">
-        <f t="shared" si="7"/>
-        <v>0.48982453512766244</v>
-      </c>
-      <c r="M21" t="str">
-        <f t="shared" ref="M21:M22" ca="1" si="8">IF(RAND()&gt;(1-E21),"yes","no")</f>
-        <v>no</v>
-      </c>
-      <c r="N21" t="str">
-        <f t="shared" ref="N21:N22" ca="1" si="9">IF(RAND()&gt;(1-F21),"yes","no")</f>
-        <v>yes</v>
-      </c>
-      <c r="O21" t="str">
-        <f t="shared" ref="O21:O22" ca="1" si="10">IF(RAND()&gt;(1-G21),"yes","no")</f>
-        <v>no</v>
-      </c>
-      <c r="P21" t="str">
-        <f t="shared" ref="P21:P22" ca="1" si="11">IF(RAND()&gt;(1-H21),"yes","no")</f>
-        <v>no</v>
-      </c>
-      <c r="Q21" t="str">
-        <f t="shared" ref="Q21:Q22" ca="1" si="12">IF(RAND()&gt;(1-I21),"yes","no")</f>
-        <v>no</v>
-      </c>
-      <c r="R21" t="str">
-        <f t="shared" ref="R21:R22" ca="1" si="13">IF(RAND()&gt;(1-J21),"yes","no")</f>
-        <v>no</v>
-      </c>
-      <c r="T21" t="s">
-        <v>38</v>
-      </c>
-      <c r="U21">
-        <f ca="1">COUNTIF(M26:R28,"yes")</f>
         <v>12</v>
       </c>
-      <c r="V21">
-        <f ca="1">COUNTIF(M26:R28,"no")</f>
-        <v>6</v>
-      </c>
-      <c r="W21">
-        <f t="shared" ca="1" si="6"/>
-        <v>66.666666666666657</v>
-      </c>
-    </row>
-    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="X21">
+        <f t="shared" ref="X21:X23" ca="1" si="13">V21/(V21+W21)*100</f>
+        <v>33.333333333333329</v>
+      </c>
+    </row>
+    <row r="22" spans="2:24" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E22" s="7">
         <f t="shared" ref="E22:J22" si="14">$E$18*D15</f>
@@ -1076,71 +1090,71 @@
         <v>0.38785514498187862</v>
       </c>
       <c r="M22" t="str">
+        <f t="shared" ca="1" si="7"/>
+        <v>no</v>
+      </c>
+      <c r="N22" t="str">
         <f t="shared" ca="1" si="8"/>
         <v>no</v>
       </c>
-      <c r="N22" t="str">
+      <c r="O22" t="str">
         <f t="shared" ca="1" si="9"/>
         <v>yes</v>
       </c>
-      <c r="O22" t="str">
+      <c r="P22" t="str">
         <f t="shared" ca="1" si="10"/>
-        <v>yes</v>
-      </c>
-      <c r="P22" t="str">
+        <v>no</v>
+      </c>
+      <c r="Q22" t="str">
         <f t="shared" ca="1" si="11"/>
         <v>no</v>
       </c>
-      <c r="Q22" t="str">
+      <c r="R22" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>yes</v>
-      </c>
-      <c r="R22" t="str">
+        <v>no</v>
+      </c>
+      <c r="U22" t="s">
+        <v>35</v>
+      </c>
+      <c r="V22">
+        <f ca="1">COUNTIF(M26:R28,"yes")</f>
+        <v>10</v>
+      </c>
+      <c r="W22">
+        <f ca="1">COUNTIF(M26:R28,"no")</f>
+        <v>8</v>
+      </c>
+      <c r="X22">
         <f t="shared" ca="1" si="13"/>
-        <v>yes</v>
-      </c>
-      <c r="T22" t="s">
-        <v>39</v>
-      </c>
-      <c r="U22">
-        <f ca="1">COUNTIF(M32:R34,"yes")</f>
-        <v>11</v>
-      </c>
-      <c r="V22">
-        <f ca="1">COUNTIF(M32:R34,"no")</f>
-        <v>7</v>
-      </c>
-      <c r="W22">
-        <f t="shared" ca="1" si="6"/>
-        <v>61.111111111111114</v>
-      </c>
-    </row>
-    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
+        <v>55.555555555555557</v>
+      </c>
+    </row>
+    <row r="23" spans="2:24" x14ac:dyDescent="0.25">
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
-      <c r="T23" t="s">
+      <c r="U23" t="s">
         <v>36</v>
       </c>
-      <c r="U23">
-        <f ca="1">COUNTIF(M20:R34,"yes")</f>
-        <v>32</v>
-      </c>
       <c r="V23">
-        <f ca="1">COUNTIF(M20:R34,"no")</f>
-        <v>22</v>
+        <f ca="1">COUNTIF(M32:R34,"yes")</f>
+        <v>12</v>
       </c>
       <c r="W23">
-        <f ca="1">U23/(U23+V23)*100</f>
-        <v>59.259259259259252</v>
-      </c>
-    </row>
-    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
+        <f ca="1">COUNTIF(M32:R34,"no")</f>
+        <v>6</v>
+      </c>
+      <c r="X23">
+        <f t="shared" ca="1" si="13"/>
+        <v>66.666666666666657</v>
+      </c>
+    </row>
+    <row r="24" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B24" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
@@ -1152,36 +1166,51 @@
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
-    </row>
-    <row r="25" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="U24" t="s">
+        <v>33</v>
+      </c>
+      <c r="V24">
+        <f ca="1">COUNTIF(M20:R34,"yes")</f>
+        <v>28</v>
+      </c>
+      <c r="W24">
+        <f ca="1">COUNTIF(M20:R34,"no")</f>
+        <v>26</v>
+      </c>
+      <c r="X24">
+        <f ca="1">V24/(V24+W24)*100</f>
+        <v>51.851851851851848</v>
+      </c>
+    </row>
+    <row r="25" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F25" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G25" s="7" t="s">
+      <c r="I25" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H25" s="7" t="s">
+      <c r="J25" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I25" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J25" s="7" t="s">
-        <v>22</v>
-      </c>
       <c r="M25" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="2:24" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E26" s="7">
         <f>$E$24*D13</f>
@@ -1221,7 +1250,7 @@
       </c>
       <c r="P26" t="str">
         <f t="shared" ref="P26:P34" ca="1" si="19">IF(RAND()&gt;(1-H26),"yes","no")</f>
-        <v>yes</v>
+        <v>no</v>
       </c>
       <c r="Q26" t="str">
         <f t="shared" ref="Q26:Q34" ca="1" si="20">IF(RAND()&gt;(1-I26),"yes","no")</f>
@@ -1232,9 +1261,9 @@
         <v>yes</v>
       </c>
     </row>
-    <row r="27" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:24" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E27" s="7">
         <f t="shared" ref="E27:J27" si="22">$E$24*D14</f>
@@ -1262,32 +1291,32 @@
       </c>
       <c r="M27" t="str">
         <f t="shared" ca="1" si="16"/>
-        <v>yes</v>
+        <v>no</v>
       </c>
       <c r="N27" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>no</v>
+        <v>yes</v>
       </c>
       <c r="O27" t="str">
         <f t="shared" ca="1" si="18"/>
-        <v>yes</v>
+        <v>no</v>
       </c>
       <c r="P27" t="str">
         <f t="shared" ca="1" si="19"/>
-        <v>no</v>
+        <v>yes</v>
       </c>
       <c r="Q27" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>yes</v>
+        <v>no</v>
       </c>
       <c r="R27" t="str">
         <f t="shared" ca="1" si="21"/>
-        <v>no</v>
-      </c>
-    </row>
-    <row r="28" spans="2:23" x14ac:dyDescent="0.25">
+        <v>yes</v>
+      </c>
+    </row>
+    <row r="28" spans="2:24" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E28" s="7">
         <f t="shared" ref="E28:J28" si="23">$E$24*D15</f>
@@ -1315,30 +1344,30 @@
       </c>
       <c r="M28" t="str">
         <f t="shared" ca="1" si="16"/>
-        <v>yes</v>
+        <v>no</v>
       </c>
       <c r="N28" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>no</v>
+        <v>yes</v>
       </c>
       <c r="O28" t="str">
         <f t="shared" ca="1" si="18"/>
-        <v>no</v>
+        <v>yes</v>
       </c>
       <c r="P28" t="str">
         <f t="shared" ca="1" si="19"/>
-        <v>yes</v>
+        <v>no</v>
       </c>
       <c r="Q28" t="str">
         <f t="shared" ca="1" si="20"/>
-        <v>yes</v>
+        <v>no</v>
       </c>
       <c r="R28" t="str">
         <f t="shared" ca="1" si="21"/>
         <v>no</v>
       </c>
     </row>
-    <row r="29" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:24" x14ac:dyDescent="0.25">
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
@@ -1346,9 +1375,9 @@
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
     </row>
-    <row r="30" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B30" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
@@ -1361,35 +1390,35 @@
       <c r="I30" s="7"/>
       <c r="J30" s="7"/>
     </row>
-    <row r="31" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F31" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H31" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G31" s="7" t="s">
+      <c r="I31" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H31" s="7" t="s">
+      <c r="J31" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I31" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J31" s="7" t="s">
-        <v>22</v>
-      </c>
       <c r="M31" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="32" spans="2:23" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="2:24" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E32" s="7">
         <f>$E$30*D13</f>
@@ -1421,7 +1450,7 @@
       </c>
       <c r="N32" t="str">
         <f t="shared" ca="1" si="17"/>
-        <v>no</v>
+        <v>yes</v>
       </c>
       <c r="O32" t="str">
         <f t="shared" ca="1" si="18"/>
@@ -1437,12 +1466,12 @@
       </c>
       <c r="R32" t="str">
         <f t="shared" ca="1" si="21"/>
-        <v>yes</v>
+        <v>no</v>
       </c>
     </row>
     <row r="33" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D33" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E33" s="7">
         <f t="shared" ref="E33:J33" si="25">$E$30*D14</f>
@@ -1470,7 +1499,7 @@
       </c>
       <c r="M33" t="str">
         <f t="shared" ca="1" si="16"/>
-        <v>yes</v>
+        <v>no</v>
       </c>
       <c r="N33" t="str">
         <f t="shared" ca="1" si="17"/>
@@ -1482,7 +1511,7 @@
       </c>
       <c r="P33" t="str">
         <f t="shared" ca="1" si="19"/>
-        <v>no</v>
+        <v>yes</v>
       </c>
       <c r="Q33" t="str">
         <f t="shared" ca="1" si="20"/>
@@ -1495,7 +1524,7 @@
     </row>
     <row r="34" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E34" s="7">
         <f t="shared" ref="E34:J34" si="26">$E$30*D15</f>
@@ -1531,7 +1560,7 @@
       </c>
       <c r="O34" t="str">
         <f t="shared" ca="1" si="18"/>
-        <v>no</v>
+        <v>yes</v>
       </c>
       <c r="P34" t="str">
         <f t="shared" ca="1" si="19"/>
@@ -1553,11 +1582,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="H1:K1"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="E3:G3"/>
-    <mergeCell ref="E4:G4"/>
     <mergeCell ref="B30:D30"/>
     <mergeCell ref="H3:K3"/>
     <mergeCell ref="H4:K4"/>
@@ -1566,6 +1590,11 @@
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E4:G4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>